<commit_message>
12 instructions test pass
</commit_message>
<xml_diff>
--- a/Simple Instruction Set 1.xlsx
+++ b/Simple Instruction Set 1.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="64">
   <si>
     <t>nop</t>
   </si>
@@ -90,51 +90,15 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>mov A, #hF0</t>
-  </si>
-  <si>
     <t>sta h02</t>
   </si>
   <si>
     <t>loop:</t>
   </si>
   <si>
-    <t>dec  h01</t>
-  </si>
-  <si>
-    <t>jn exit</t>
-  </si>
-  <si>
     <t>jmp loop</t>
   </si>
   <si>
-    <t>exit</t>
-  </si>
-  <si>
-    <t>тело цикла</t>
-  </si>
-  <si>
-    <t>количество итераций</t>
-  </si>
-  <si>
-    <t>шаг цикла</t>
-  </si>
-  <si>
-    <t>lda h02</t>
-  </si>
-  <si>
-    <t>загружаем итерации</t>
-  </si>
-  <si>
-    <t>вычитаем шаг</t>
-  </si>
-  <si>
-    <t>если все, то конец</t>
-  </si>
-  <si>
-    <t>в начало цикла</t>
-  </si>
-  <si>
     <t>остановка</t>
   </si>
   <si>
@@ -153,7 +117,97 @@
     <t>Набор инструкций для процессора гарвардской архитектуры</t>
   </si>
   <si>
-    <t>сохраняем итерации</t>
+    <t>a</t>
+  </si>
+  <si>
+    <t>mov A,#7</t>
+  </si>
+  <si>
+    <t>sta h00</t>
+  </si>
+  <si>
+    <t>ячейка 0</t>
+  </si>
+  <si>
+    <t>mov A, #h04</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>mov A,#6</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>mov A,#0</t>
+  </si>
+  <si>
+    <t>res</t>
+  </si>
+  <si>
+    <t>ячейка 3</t>
+  </si>
+  <si>
+    <t>sta h03</t>
+  </si>
+  <si>
+    <t>sta h04</t>
+  </si>
+  <si>
+    <t>ячейка 4</t>
+  </si>
+  <si>
+    <t>lda h03</t>
+  </si>
+  <si>
+    <t>загрузить res</t>
+  </si>
+  <si>
+    <t>add h00</t>
+  </si>
+  <si>
+    <t>res+=a</t>
+  </si>
+  <si>
+    <t>lda h01</t>
+  </si>
+  <si>
+    <t>сохранить res</t>
+  </si>
+  <si>
+    <t>згрузить x</t>
+  </si>
+  <si>
+    <t>dec h04</t>
+  </si>
+  <si>
+    <t>x-=1</t>
+  </si>
+  <si>
+    <t>сохранить x</t>
+  </si>
+  <si>
+    <t>jz exit</t>
+  </si>
+  <si>
+    <t>выход если x=0</t>
+  </si>
+  <si>
+    <t>еще цикл</t>
+  </si>
+  <si>
+    <t>add h02</t>
+  </si>
+  <si>
+    <t>res+=b</t>
+  </si>
+  <si>
+    <t>exit:</t>
+  </si>
+  <si>
+    <t>шаг цикла 1</t>
   </si>
 </sst>
 </file>
@@ -647,10 +701,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:AI27"/>
+  <dimension ref="B2:AI43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="N37" sqref="N37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -692,7 +746,7 @@
   <sheetData>
     <row r="2" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B2" s="12" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="C2" s="12"/>
       <c r="D2" s="12"/>
@@ -932,7 +986,7 @@
     </row>
     <row r="9" spans="2:35" x14ac:dyDescent="0.25">
       <c r="Y9" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="Z9" t="s">
         <v>7</v>
@@ -1050,7 +1104,7 @@
     </row>
     <row r="14" spans="2:35" x14ac:dyDescent="0.25">
       <c r="L14" s="9" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="N14" s="2">
         <v>1</v>
@@ -1072,14 +1126,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="2:35" x14ac:dyDescent="0.25">
-      <c r="K15" t="s">
-        <v>0</v>
-      </c>
-    </row>
     <row r="16" spans="2:35" x14ac:dyDescent="0.25">
       <c r="K16" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="L16" s="9" t="s">
         <v>33</v>
@@ -1106,10 +1155,10 @@
     </row>
     <row r="17" spans="10:12" x14ac:dyDescent="0.25">
       <c r="K17" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="L17" s="9" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="10:12" x14ac:dyDescent="0.25">
@@ -1117,78 +1166,178 @@
         <v>23</v>
       </c>
       <c r="K18" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="L18" s="9" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="10:12" x14ac:dyDescent="0.25">
       <c r="K19" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="L19" s="9" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="10:12" x14ac:dyDescent="0.25">
-      <c r="J20" t="s">
-        <v>26</v>
-      </c>
       <c r="K20" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="L20" s="9" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="10:12" x14ac:dyDescent="0.25">
       <c r="K21" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="L21" s="9" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="10:12" x14ac:dyDescent="0.25">
       <c r="K22" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="L22" s="9" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="10:12" x14ac:dyDescent="0.25">
       <c r="K23" t="s">
+        <v>44</v>
+      </c>
+      <c r="L23" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="K24" t="s">
+        <v>21</v>
+      </c>
+      <c r="L24" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="K25" t="s">
+        <v>45</v>
+      </c>
+      <c r="L25" s="9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="J26" t="s">
         <v>25</v>
       </c>
-      <c r="L23" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="24" spans="10:12" x14ac:dyDescent="0.25">
-      <c r="L24" s="9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="26" spans="10:12" x14ac:dyDescent="0.25">
       <c r="K26" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="L26" s="9" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="10:12" x14ac:dyDescent="0.25">
-      <c r="J27" t="s">
-        <v>30</v>
-      </c>
       <c r="K27" t="s">
+        <v>49</v>
+      </c>
+      <c r="L27" s="9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="K28" t="s">
+        <v>44</v>
+      </c>
+      <c r="L28" s="9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="J29" t="s">
+        <v>23</v>
+      </c>
+      <c r="K29" t="s">
+        <v>51</v>
+      </c>
+      <c r="L29" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="30" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="K30" t="s">
+        <v>54</v>
+      </c>
+      <c r="L30" s="9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="K31" t="s">
+        <v>22</v>
+      </c>
+      <c r="L31" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="32" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="K32" t="s">
+        <v>57</v>
+      </c>
+      <c r="L32" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="33" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="K33" t="s">
+        <v>26</v>
+      </c>
+      <c r="L33" s="9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="J34" t="s">
+        <v>62</v>
+      </c>
+      <c r="K34" t="s">
+        <v>47</v>
+      </c>
+      <c r="L34" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="35" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="K35" t="s">
+        <v>60</v>
+      </c>
+      <c r="L35" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="36" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="K36" t="s">
+        <v>44</v>
+      </c>
+      <c r="L36" s="9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="37" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="K37" t="s">
         <v>3</v>
       </c>
-      <c r="L27" s="9" t="s">
-        <v>39</v>
-      </c>
+      <c r="L37" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="42" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="L42" s="9"/>
+    </row>
+    <row r="43" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="L43" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>